<commit_message>
updating excel files and local postgres db
</commit_message>
<xml_diff>
--- a/Resources/hours_per_week_by_country.xlsx
+++ b/Resources/hours_per_week_by_country.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcbie\RICE_BOOTCAMP\Working Folder\Project_Two\Project-2\data\gamer stat percentages by country, age, gender\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sadie\Documents\Data Analytics Coursework\Project#2.5\Project-2\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7ABFC0-B550-44E2-B60B-635BBAAA2884}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B7524A-1DE4-4AD1-87E5-434C51877427}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2490" yWindow="3510" windowWidth="21600" windowHeight="11505" xr2:uid="{100434AC-E4E9-4759-8909-5AFC1781627A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{100434AC-E4E9-4759-8909-5AFC1781627A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,15 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -81,16 +72,16 @@
     <t>South Korea</t>
   </si>
   <si>
-    <t>U.K.</t>
-  </si>
-  <si>
-    <t>U.S.</t>
-  </si>
-  <si>
     <t>Global</t>
   </si>
   <si>
     <t>Average Hours Each Week</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>United States</t>
   </si>
 </sst>
 </file>
@@ -453,7 +444,7 @@
   <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,7 +475,7 @@
         <v>8</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -788,7 +779,7 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1">
         <v>0.154</v>
@@ -829,7 +820,7 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B10" s="1">
         <v>0.128</v>
@@ -870,7 +861,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B11" s="1">
         <v>0.14899999999999999</v>

</xml_diff>